<commit_message>
Use 2% GDP growth for both BAU and alternate values for GDPGR
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-texas\InputData\ctrl-settings\GDPGR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\EI-eps-texas\InputData\ctrl-settings\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="GDPGR-alternate" sheetId="2" r:id="rId3"/>
     <sheet name="GDPGR-bau" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1160,7 +1160,8 @@
         <v>27</v>
       </c>
       <c r="B2" s="22">
-        <v>0</v>
+        <f>Data!B11</f>
+        <v>1.9928676316341543E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1197,7 +1198,8 @@
         <v>29</v>
       </c>
       <c r="B2" s="22">
-        <v>0</v>
+        <f>Data!B11</f>
+        <v>1.9928676316341543E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>